<commit_message>
resolved some issues when pressure varies
bugs stopped running of simulations when pressure varied with time. now resolved.
</commit_message>
<xml_diff>
--- a/PyCHAM/input/guaiacol/constraining_obs.xlsx
+++ b/PyCHAM/input/guaiacol/constraining_obs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/PyCHAM/PyCHAM/input/guaiacol/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C72C95-6944-B640-8E10-7B2F2BA384A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F25E375-1FEF-724A-8D1A-B48B16EAF9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10480" yWindow="7020" windowWidth="21380" windowHeight="13220" activeTab="1" xr2:uid="{7C74D523-2B60-6A4A-ACEB-A35EBE6838C7}"/>
+    <workbookView xWindow="6560" yWindow="3420" windowWidth="20720" windowHeight="10440" activeTab="1" xr2:uid="{7C74D523-2B60-6A4A-ACEB-A35EBE6838C7}"/>
   </bookViews>
   <sheets>
     <sheet name="ex" sheetId="1" r:id="rId1"/>
     <sheet name="PyCHAMobs" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="J4_" localSheetId="1">PyCHAMobs!$H$2:$I$72</definedName>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Time (s)</t>
   </si>
@@ -104,6 +105,12 @@
   </si>
   <si>
     <t>HONO</t>
+  </si>
+  <si>
+    <t>GUAIACOL</t>
+  </si>
+  <si>
+    <t>HCHO</t>
   </si>
 </sst>
 </file>
@@ -167,15 +174,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="TEMP" connectionId="3" xr16:uid="{D0065C49-588C-824D-AC9C-7AE07CFA4951}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="J4" connectionId="1" xr16:uid="{F0DAC9DC-9730-B148-A986-493A8A43F5B7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="J4" connectionId="1" xr16:uid="{F0DAC9DC-9730-B148-A986-493A8A43F5B7}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RH" connectionId="2" xr16:uid="{40937839-10CF-B04D-ACC8-BC40CEA32DF3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RH" connectionId="2" xr16:uid="{40937839-10CF-B04D-ACC8-BC40CEA32DF3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="TEMP" connectionId="3" xr16:uid="{D0065C49-588C-824D-AC9C-7AE07CFA4951}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3825,13 +3832,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172C4B10-34B1-DA4C-872D-C5918B25BFA3}">
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H92"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:O1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
@@ -3841,7 +3848,7 @@
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3866,8 +3873,20 @@
       <c r="H1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3892,9 +3911,20 @@
       <c r="H2" s="2">
         <v>436000000000</v>
       </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I2" s="1">
+        <v>10900000000000</v>
+      </c>
+      <c r="J2">
+        <v>1758465644</v>
+      </c>
+      <c r="K2" s="1">
+        <v>888000000000</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1050000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>60</v>
       </c>
@@ -3919,8 +3949,20 @@
       <c r="H3" s="2">
         <v>562800000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I3">
+        <v>10574000000000</v>
+      </c>
+      <c r="J3">
+        <v>1758465644</v>
+      </c>
+      <c r="K3" s="1">
+        <v>906000000000</v>
+      </c>
+      <c r="L3" s="1">
+        <v>988000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>120</v>
       </c>
@@ -3945,8 +3987,20 @@
       <c r="H4" s="2">
         <v>689600000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I4">
+        <v>10248000000000</v>
+      </c>
+      <c r="J4">
+        <v>1758465644</v>
+      </c>
+      <c r="K4" s="1">
+        <v>930000000000</v>
+      </c>
+      <c r="L4" s="1">
+        <v>934000000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>180</v>
       </c>
@@ -3971,8 +4025,20 @@
       <c r="H5" s="2">
         <v>816400000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5">
+        <v>9922000000000</v>
+      </c>
+      <c r="J5">
+        <v>1758465644</v>
+      </c>
+      <c r="K5" s="1">
+        <v>892000000000</v>
+      </c>
+      <c r="L5" s="1">
+        <v>984000000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>240</v>
       </c>
@@ -3997,8 +4063,20 @@
       <c r="H6" s="2">
         <v>943200000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I6">
+        <v>9596000000000</v>
+      </c>
+      <c r="J6">
+        <v>1758465644</v>
+      </c>
+      <c r="K6" s="1">
+        <v>831000000000</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1050000000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>300</v>
       </c>
@@ -4023,8 +4101,20 @@
       <c r="H7" s="2">
         <v>1070000000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I7">
+        <v>9270000000000</v>
+      </c>
+      <c r="J7">
+        <v>1758465644</v>
+      </c>
+      <c r="K7" s="1">
+        <v>754000000000</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1120000000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>360</v>
       </c>
@@ -4049,8 +4139,20 @@
       <c r="H8" s="2">
         <v>1188000000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>9016000000000</v>
+      </c>
+      <c r="J8">
+        <v>9056967018</v>
+      </c>
+      <c r="K8" s="1">
+        <v>692000000000</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1180000000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>420</v>
       </c>
@@ -4075,8 +4177,20 @@
       <c r="H9" s="2">
         <v>1306000000000</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>8762000000000</v>
+      </c>
+      <c r="J9">
+        <v>16167990656</v>
+      </c>
+      <c r="K9" s="1">
+        <v>651000000000</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1250000000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>480</v>
       </c>
@@ -4101,8 +4215,20 @@
       <c r="H10" s="2">
         <v>1424000000000</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>8508000000000</v>
+      </c>
+      <c r="J10">
+        <v>24617300084</v>
+      </c>
+      <c r="K10" s="1">
+        <v>609000000000</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1280000000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>540</v>
       </c>
@@ -4127,8 +4253,20 @@
       <c r="H11" s="2">
         <v>1542000000000</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>8254000000000</v>
+      </c>
+      <c r="J11">
+        <v>33123658774</v>
+      </c>
+      <c r="K11" s="1">
+        <v>555000000000</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1310000000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>600</v>
       </c>
@@ -4153,8 +4291,20 @@
       <c r="H12" s="2">
         <v>1660000000000</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>8000000000000</v>
+      </c>
+      <c r="J12">
+        <v>41499412781</v>
+      </c>
+      <c r="K12" s="1">
+        <v>518000000000</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1330000000000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>660</v>
       </c>
@@ -4179,8 +4329,20 @@
       <c r="H13" s="2">
         <v>1756000000000</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>7774000000000</v>
+      </c>
+      <c r="J13">
+        <v>50468705728</v>
+      </c>
+      <c r="K13" s="1">
+        <v>504000000000</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1340000000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>720</v>
       </c>
@@ -4205,8 +4367,20 @@
       <c r="H14" s="2">
         <v>1852000000000</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I14">
+        <v>7548000000000</v>
+      </c>
+      <c r="J14">
+        <v>60686968653</v>
+      </c>
+      <c r="K14" s="1">
+        <v>473000000000</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1350000000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>780</v>
       </c>
@@ -4231,8 +4405,20 @@
       <c r="H15" s="2">
         <v>1948000000000</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I15">
+        <v>7322000000000</v>
+      </c>
+      <c r="J15">
+        <v>70490484996</v>
+      </c>
+      <c r="K15" s="1">
+        <v>437000000000</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1340000000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>840</v>
       </c>
@@ -4257,8 +4443,20 @@
       <c r="H16" s="2">
         <v>2044000000000</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16">
+        <v>7096000000000</v>
+      </c>
+      <c r="J16">
+        <v>79871811884</v>
+      </c>
+      <c r="K16" s="1">
+        <v>413000000000</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1350000000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>900</v>
       </c>
@@ -4283,8 +4481,20 @@
       <c r="H17" s="2">
         <v>2140000000000</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17">
+        <v>6870000000000</v>
+      </c>
+      <c r="J17">
+        <v>91996741205</v>
+      </c>
+      <c r="K17" s="1">
+        <v>391000000000</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1340000000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>960</v>
       </c>
@@ -4309,8 +4519,20 @@
       <c r="H18" s="2">
         <v>2208000000000</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18">
+        <v>6670000000000</v>
+      </c>
+      <c r="J18">
+        <v>102537000000</v>
+      </c>
+      <c r="K18" s="1">
+        <v>369000000000</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1340000000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1020</v>
       </c>
@@ -4335,8 +4557,20 @@
       <c r="H19" s="2">
         <v>2276000000000</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>6470000000000</v>
+      </c>
+      <c r="J19">
+        <v>112486000000</v>
+      </c>
+      <c r="K19" s="1">
+        <v>353000000000</v>
+      </c>
+      <c r="L19" s="1">
+        <v>1320000000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1080</v>
       </c>
@@ -4361,8 +4595,20 @@
       <c r="H20" s="2">
         <v>2344000000000</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20">
+        <v>6270000000000</v>
+      </c>
+      <c r="J20">
+        <v>126114000000</v>
+      </c>
+      <c r="K20" s="1">
+        <v>349000000000</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1310000000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1140</v>
       </c>
@@ -4387,8 +4633,20 @@
       <c r="H21" s="2">
         <v>2412000000000</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21">
+        <v>6070000000000</v>
+      </c>
+      <c r="J21">
+        <v>146740000000</v>
+      </c>
+      <c r="K21" s="1">
+        <v>348000000000</v>
+      </c>
+      <c r="L21" s="1">
+        <v>1300000000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1200</v>
       </c>
@@ -4413,8 +4671,20 @@
       <c r="H22" s="2">
         <v>2480000000000</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22">
+        <v>5870000000000</v>
+      </c>
+      <c r="J22">
+        <v>158982000000</v>
+      </c>
+      <c r="K22" s="1">
+        <v>344000000000</v>
+      </c>
+      <c r="L22" s="1">
+        <v>1290000000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1260</v>
       </c>
@@ -4439,8 +4709,20 @@
       <c r="H23" s="2">
         <v>2544000000000</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23">
+        <v>5696000000000</v>
+      </c>
+      <c r="J23">
+        <v>165527000000</v>
+      </c>
+      <c r="K23" s="1">
+        <v>339000000000</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1270000000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1320</v>
       </c>
@@ -4465,8 +4747,20 @@
       <c r="H24" s="2">
         <v>2608000000000</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>5522000000000</v>
+      </c>
+      <c r="J24">
+        <v>188466000000</v>
+      </c>
+      <c r="K24" s="1">
+        <v>329000000000</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1250000000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1380</v>
       </c>
@@ -4491,8 +4785,20 @@
       <c r="H25" s="2">
         <v>2672000000000</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>5348000000000</v>
+      </c>
+      <c r="J25">
+        <v>201501000000</v>
+      </c>
+      <c r="K25" s="1">
+        <v>318000000000</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1230000000000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1440</v>
       </c>
@@ -4517,8 +4823,20 @@
       <c r="H26" s="2">
         <v>2736000000000</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26">
+        <v>5174000000000</v>
+      </c>
+      <c r="J26">
+        <v>206117000000</v>
+      </c>
+      <c r="K26" s="1">
+        <v>308000000000</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1220000000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1500</v>
       </c>
@@ -4543,8 +4861,20 @@
       <c r="H27" s="2">
         <v>2800000000000</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>5000000000000</v>
+      </c>
+      <c r="J27">
+        <v>213442000000</v>
+      </c>
+      <c r="K27" s="1">
+        <v>295000000000</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1220000000000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1560</v>
       </c>
@@ -4569,8 +4899,20 @@
       <c r="H28" s="2">
         <v>2850000000000</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28">
+        <v>4872000000000</v>
+      </c>
+      <c r="J28">
+        <v>220717000000</v>
+      </c>
+      <c r="K28" s="1">
+        <v>281000000000</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1210000000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1620</v>
       </c>
@@ -4595,8 +4937,20 @@
       <c r="H29" s="2">
         <v>2900000000000</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>4744000000000</v>
+      </c>
+      <c r="J29">
+        <v>228777000000</v>
+      </c>
+      <c r="K29" s="1">
+        <v>270000000000</v>
+      </c>
+      <c r="L29" s="1">
+        <v>1170000000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1680</v>
       </c>
@@ -4621,8 +4975,20 @@
       <c r="H30" s="2">
         <v>2950000000000</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30">
+        <v>4616000000000</v>
+      </c>
+      <c r="J30">
+        <v>237628000000</v>
+      </c>
+      <c r="K30" s="1">
+        <v>260000000000</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1150000000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1740</v>
       </c>
@@ -4647,8 +5013,20 @@
       <c r="H31" s="2">
         <v>3000000000000</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <v>4488000000000</v>
+      </c>
+      <c r="J31">
+        <v>255626000000</v>
+      </c>
+      <c r="K31" s="1">
+        <v>246000000000</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1130000000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1800</v>
       </c>
@@ -4673,8 +5051,20 @@
       <c r="H32" s="2">
         <v>3050000000000</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32">
+        <v>4360000000000</v>
+      </c>
+      <c r="J32">
+        <v>258358000000</v>
+      </c>
+      <c r="K32" s="1">
+        <v>238000000000</v>
+      </c>
+      <c r="L32" s="1">
+        <v>1110000000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1860</v>
       </c>
@@ -4699,8 +5089,20 @@
       <c r="H33" s="2">
         <v>3096000000000</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33">
+        <v>4256000000000</v>
+      </c>
+      <c r="J33">
+        <v>259209000000</v>
+      </c>
+      <c r="K33" s="1">
+        <v>230000000000</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1090000000000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1920</v>
       </c>
@@ -4725,8 +5127,20 @@
       <c r="H34" s="2">
         <v>3142000000000</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34">
+        <v>4152000000000</v>
+      </c>
+      <c r="J34">
+        <v>261623000000</v>
+      </c>
+      <c r="K34" s="1">
+        <v>220000000000</v>
+      </c>
+      <c r="L34" s="1">
+        <v>1070000000000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1980</v>
       </c>
@@ -4751,8 +5165,20 @@
       <c r="H35" s="2">
         <v>3188000000000</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35">
+        <v>4048000000000</v>
+      </c>
+      <c r="J35">
+        <v>268158000000</v>
+      </c>
+      <c r="K35" s="1">
+        <v>215000000000</v>
+      </c>
+      <c r="L35" s="1">
+        <v>1050000000000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2040</v>
       </c>
@@ -4777,8 +5203,20 @@
       <c r="H36" s="2">
         <v>3234000000000</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36">
+        <v>3944000000000</v>
+      </c>
+      <c r="J36">
+        <v>282585000000</v>
+      </c>
+      <c r="K36" s="1">
+        <v>208000000000</v>
+      </c>
+      <c r="L36" s="1">
+        <v>1030000000000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2100</v>
       </c>
@@ -4803,8 +5241,20 @@
       <c r="H37" s="2">
         <v>3280000000000</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37">
+        <v>3840000000000</v>
+      </c>
+      <c r="J37">
+        <v>298319000000</v>
+      </c>
+      <c r="K37" s="1">
+        <v>201000000000</v>
+      </c>
+      <c r="L37" s="1">
+        <v>1010000000000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2160</v>
       </c>
@@ -4829,8 +5279,20 @@
       <c r="H38" s="2">
         <v>3318000000000</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38">
+        <v>3750000000000</v>
+      </c>
+      <c r="J38">
+        <v>301686000000</v>
+      </c>
+      <c r="K38" s="1">
+        <v>194000000000</v>
+      </c>
+      <c r="L38" s="1">
+        <v>991000000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2220</v>
       </c>
@@ -4855,8 +5317,20 @@
       <c r="H39" s="2">
         <v>3356000000000</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39">
+        <v>3660000000000</v>
+      </c>
+      <c r="J39">
+        <v>303747000000</v>
+      </c>
+      <c r="K39" s="1">
+        <v>186000000000</v>
+      </c>
+      <c r="L39" s="1">
+        <v>960000000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2340</v>
       </c>
@@ -4881,8 +5355,20 @@
       <c r="H40" s="2">
         <v>3432000000000</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40">
+        <v>3480000000000</v>
+      </c>
+      <c r="J40">
+        <v>326838000000</v>
+      </c>
+      <c r="K40" s="1">
+        <v>173000000000</v>
+      </c>
+      <c r="L40" s="1">
+        <v>934000000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2400</v>
       </c>
@@ -4907,8 +5393,20 @@
       <c r="H41" s="2">
         <v>3470000000000</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41">
+        <v>3390000000000</v>
+      </c>
+      <c r="J41">
+        <v>370110000000</v>
+      </c>
+      <c r="K41" s="1">
+        <v>167000000000</v>
+      </c>
+      <c r="L41" s="1">
+        <v>917000000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2460</v>
       </c>
@@ -4933,8 +5431,20 @@
       <c r="H42" s="2">
         <v>3502000000000</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42">
+        <v>3314000000000</v>
+      </c>
+      <c r="J42">
+        <v>383311000000</v>
+      </c>
+      <c r="K42" s="1">
+        <v>159000000000</v>
+      </c>
+      <c r="L42" s="1">
+        <v>899000000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2520</v>
       </c>
@@ -4959,8 +5469,20 @@
       <c r="H43" s="2">
         <v>3534000000000</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43">
+        <v>3238000000000</v>
+      </c>
+      <c r="J43">
+        <v>369750000000</v>
+      </c>
+      <c r="K43" s="1">
+        <v>155000000000</v>
+      </c>
+      <c r="L43" s="1">
+        <v>880000000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2580</v>
       </c>
@@ -4985,8 +5507,20 @@
       <c r="H44" s="2">
         <v>3566000000000</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44">
+        <v>3162000000000</v>
+      </c>
+      <c r="J44">
+        <v>364267000000</v>
+      </c>
+      <c r="K44" s="1">
+        <v>148000000000</v>
+      </c>
+      <c r="L44" s="1">
+        <v>863000000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2640</v>
       </c>
@@ -5011,8 +5545,20 @@
       <c r="H45" s="2">
         <v>3598000000000</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45">
+        <v>3086000000000</v>
+      </c>
+      <c r="J45">
+        <v>363907000000</v>
+      </c>
+      <c r="K45" s="1">
+        <v>143000000000</v>
+      </c>
+      <c r="L45" s="1">
+        <v>846000000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2700</v>
       </c>
@@ -5037,8 +5583,20 @@
       <c r="H46" s="2">
         <v>3630000000000</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46">
+        <v>3010000000000</v>
+      </c>
+      <c r="J46">
+        <v>369246000000</v>
+      </c>
+      <c r="K46" s="1">
+        <v>138000000000</v>
+      </c>
+      <c r="L46" s="1">
+        <v>826000000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2760</v>
       </c>
@@ -5063,8 +5621,20 @@
       <c r="H47" s="2">
         <v>3651666666666.6602</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47">
+        <v>2956666666666.6602</v>
+      </c>
+      <c r="J47">
+        <v>387357000000</v>
+      </c>
+      <c r="K47" s="1">
+        <v>137000000000</v>
+      </c>
+      <c r="L47" s="1">
+        <v>809000000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2820</v>
       </c>
@@ -5089,8 +5659,20 @@
       <c r="H48" s="2">
         <v>3673333333333.3301</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48">
+        <v>2903333333333.3301</v>
+      </c>
+      <c r="J48">
+        <v>401610000000</v>
+      </c>
+      <c r="K48" s="1">
+        <v>132000000000</v>
+      </c>
+      <c r="L48" s="1">
+        <v>792000000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2880</v>
       </c>
@@ -5115,8 +5697,20 @@
       <c r="H49" s="2">
         <v>3695000000000</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49">
+        <v>2850000000000</v>
+      </c>
+      <c r="J49">
+        <v>406518000000</v>
+      </c>
+      <c r="K49" s="1">
+        <v>130000000000</v>
+      </c>
+      <c r="L49" s="1">
+        <v>766000000000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2940</v>
       </c>
@@ -5141,8 +5735,20 @@
       <c r="H50" s="2">
         <v>3716666666666.6602</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50">
+        <v>2796666666666.6602</v>
+      </c>
+      <c r="J50">
+        <v>404686000000</v>
+      </c>
+      <c r="K50" s="1">
+        <v>124000000000</v>
+      </c>
+      <c r="L50" s="1">
+        <v>754000000000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>3000</v>
       </c>
@@ -5167,8 +5773,20 @@
       <c r="H51" s="2">
         <v>3738333333333.3301</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51">
+        <v>2743333333333.3301</v>
+      </c>
+      <c r="J51">
+        <v>419110000000</v>
+      </c>
+      <c r="K51" s="1">
+        <v>122000000000</v>
+      </c>
+      <c r="L51" s="1">
+        <v>742000000000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>3060</v>
       </c>
@@ -5193,8 +5811,20 @@
       <c r="H52" s="2">
         <v>3760000000000</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52">
+        <v>2690000000000</v>
+      </c>
+      <c r="J52">
+        <v>429770000000</v>
+      </c>
+      <c r="K52" s="1">
+        <v>119000000000</v>
+      </c>
+      <c r="L52" s="1">
+        <v>732000000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>3120</v>
       </c>
@@ -5219,8 +5849,20 @@
       <c r="H53" s="2">
         <v>3782000000000</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53">
+        <v>2640000000000</v>
+      </c>
+      <c r="J53">
+        <v>468560000000</v>
+      </c>
+      <c r="K53" s="1">
+        <v>117000000000</v>
+      </c>
+      <c r="L53" s="1">
+        <v>715000000000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>3180</v>
       </c>
@@ -5245,8 +5887,20 @@
       <c r="H54" s="2">
         <v>3804000000000</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I54">
+        <v>2590000000000</v>
+      </c>
+      <c r="J54">
+        <v>469350000000</v>
+      </c>
+      <c r="K54" s="1">
+        <v>113000000000</v>
+      </c>
+      <c r="L54" s="1">
+        <v>701000000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>3240</v>
       </c>
@@ -5271,8 +5925,20 @@
       <c r="H55" s="2">
         <v>3826000000000</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55">
+        <v>2540000000000</v>
+      </c>
+      <c r="J55">
+        <v>456237000000</v>
+      </c>
+      <c r="K55" s="1">
+        <v>111000000000</v>
+      </c>
+      <c r="L55" s="1">
+        <v>684000000000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>3300</v>
       </c>
@@ -5297,8 +5963,20 @@
       <c r="H56" s="2">
         <v>3848000000000</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56">
+        <v>2490000000000</v>
+      </c>
+      <c r="J56">
+        <v>437304000000</v>
+      </c>
+      <c r="K56" s="1">
+        <v>105000000000</v>
+      </c>
+      <c r="L56" s="1">
+        <v>673000000000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>3360</v>
       </c>
@@ -5323,8 +6001,20 @@
       <c r="H57" s="2">
         <v>3870000000000</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57">
+        <v>2440000000000</v>
+      </c>
+      <c r="J57">
+        <v>429154000000</v>
+      </c>
+      <c r="K57" s="1">
+        <v>102000000000</v>
+      </c>
+      <c r="L57" s="1">
+        <v>667000000000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>3420</v>
       </c>
@@ -5349,8 +6039,20 @@
       <c r="H58" s="2">
         <v>3892000000000</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58">
+        <v>2396000000000</v>
+      </c>
+      <c r="J58">
+        <v>460321000000</v>
+      </c>
+      <c r="K58" s="1">
+        <v>99900000000</v>
+      </c>
+      <c r="L58" s="1">
+        <v>667000000000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>3480</v>
       </c>
@@ -5375,8 +6077,20 @@
       <c r="H59" s="2">
         <v>3914000000000</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59">
+        <v>2352000000000</v>
+      </c>
+      <c r="J59">
+        <v>477961000000</v>
+      </c>
+      <c r="K59" s="1">
+        <v>98200000000</v>
+      </c>
+      <c r="L59" s="1">
+        <v>637000000000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>3540</v>
       </c>
@@ -5401,8 +6115,20 @@
       <c r="H60" s="2">
         <v>3936000000000</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60">
+        <v>2308000000000</v>
+      </c>
+      <c r="J60">
+        <v>483417000000</v>
+      </c>
+      <c r="K60" s="1">
+        <v>96200000000</v>
+      </c>
+      <c r="L60" s="1">
+        <v>618000000000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>3600</v>
       </c>
@@ -5427,8 +6153,20 @@
       <c r="H61" s="2">
         <v>3958000000000</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61">
+        <v>2264000000000</v>
+      </c>
+      <c r="J61">
+        <v>474513000000</v>
+      </c>
+      <c r="K61" s="1">
+        <v>93500000000</v>
+      </c>
+      <c r="L61" s="1">
+        <v>603000000000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>3660</v>
       </c>
@@ -5453,8 +6191,20 @@
       <c r="H62" s="2">
         <v>3980000000000</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62">
+        <v>2220000000000</v>
+      </c>
+      <c r="J62">
+        <v>456301000000</v>
+      </c>
+      <c r="K62" s="1">
+        <v>91500000000</v>
+      </c>
+      <c r="L62" s="1">
+        <v>580000000000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>3720</v>
       </c>
@@ -5479,8 +6229,20 @@
       <c r="H63" s="2">
         <v>3994000000000</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63">
+        <v>2176000000000</v>
+      </c>
+      <c r="J63">
+        <v>453540000000</v>
+      </c>
+      <c r="K63" s="1">
+        <v>87300000000</v>
+      </c>
+      <c r="L63" s="1">
+        <v>569000000000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>3780</v>
       </c>
@@ -5505,8 +6267,20 @@
       <c r="H64" s="2">
         <v>4008000000000</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64">
+        <v>2132000000000</v>
+      </c>
+      <c r="J64">
+        <v>674240000000</v>
+      </c>
+      <c r="K64" s="1">
+        <v>85100000000</v>
+      </c>
+      <c r="L64" s="1">
+        <v>561000000000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>3840</v>
       </c>
@@ -5531,8 +6305,20 @@
       <c r="H65" s="2">
         <v>4022000000000</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65">
+        <v>2088000000000</v>
+      </c>
+      <c r="J65">
+        <v>808212000000</v>
+      </c>
+      <c r="K65" s="1">
+        <v>85100000000</v>
+      </c>
+      <c r="L65" s="1">
+        <v>550000000000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>3900</v>
       </c>
@@ -5557,8 +6343,20 @@
       <c r="H66" s="2">
         <v>4036000000000</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66">
+        <v>2044000000000</v>
+      </c>
+      <c r="J66">
+        <v>653666000000</v>
+      </c>
+      <c r="K66" s="1">
+        <v>83600000000</v>
+      </c>
+      <c r="L66" s="1">
+        <v>540000000000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>3960</v>
       </c>
@@ -5583,8 +6381,20 @@
       <c r="H67" s="2">
         <v>4050000000000</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67">
+        <v>2000000000000</v>
+      </c>
+      <c r="J67">
+        <v>547203000000</v>
+      </c>
+      <c r="K67" s="1">
+        <v>80200000000</v>
+      </c>
+      <c r="L67" s="1">
+        <v>528000000000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>4020</v>
       </c>
@@ -5609,8 +6419,20 @@
       <c r="H68" s="2">
         <v>4064000000000</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68">
+        <v>1972000000000</v>
+      </c>
+      <c r="J68">
+        <v>572195000000</v>
+      </c>
+      <c r="K68" s="1">
+        <v>77000000000</v>
+      </c>
+      <c r="L68" s="1">
+        <v>518000000000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>4080</v>
       </c>
@@ -5635,8 +6457,20 @@
       <c r="H69" s="2">
         <v>4078000000000</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69">
+        <v>1944000000000</v>
+      </c>
+      <c r="J69">
+        <v>571346000000</v>
+      </c>
+      <c r="K69" s="1">
+        <v>74500000000</v>
+      </c>
+      <c r="L69" s="1">
+        <v>517000000000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>4140</v>
       </c>
@@ -5661,8 +6495,20 @@
       <c r="H70" s="2">
         <v>4092000000000</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70">
+        <v>1916000000000</v>
+      </c>
+      <c r="J70">
+        <v>539311000000</v>
+      </c>
+      <c r="K70" s="1">
+        <v>74000000000</v>
+      </c>
+      <c r="L70" s="1">
+        <v>499000000000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>4200</v>
       </c>
@@ -5687,8 +6533,20 @@
       <c r="H71" s="2">
         <v>4106000000000</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71">
+        <v>1888000000000</v>
+      </c>
+      <c r="J71">
+        <v>518566000000</v>
+      </c>
+      <c r="K71" s="1">
+        <v>73300000000</v>
+      </c>
+      <c r="L71" s="1">
+        <v>495000000000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>4260</v>
       </c>
@@ -5713,8 +6571,20 @@
       <c r="H72" s="2">
         <v>4120000000000</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72">
+        <v>1860000000000</v>
+      </c>
+      <c r="J72">
+        <v>539746000000</v>
+      </c>
+      <c r="K72" s="1">
+        <v>72800000000</v>
+      </c>
+      <c r="L72" s="1">
+        <v>491000000000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>4320</v>
       </c>
@@ -5739,8 +6609,20 @@
       <c r="H73" s="2">
         <v>4130000000000</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73">
+        <v>1838000000000</v>
+      </c>
+      <c r="J73">
+        <v>610235000000</v>
+      </c>
+      <c r="K73" s="1">
+        <v>69600000000</v>
+      </c>
+      <c r="L73" s="1">
+        <v>470000000000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>4380</v>
       </c>
@@ -5765,8 +6647,20 @@
       <c r="H74" s="2">
         <v>4140000000000</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74">
+        <v>1816000000000</v>
+      </c>
+      <c r="J74">
+        <v>587095000000</v>
+      </c>
+      <c r="K74" s="1">
+        <v>69900000000</v>
+      </c>
+      <c r="L74" s="1">
+        <v>459000000000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>4440</v>
       </c>
@@ -5791,8 +6685,20 @@
       <c r="H75" s="2">
         <v>4150000000000</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75">
+        <v>1794000000000</v>
+      </c>
+      <c r="J75">
+        <v>546138000000</v>
+      </c>
+      <c r="K75" s="1">
+        <v>69400000000</v>
+      </c>
+      <c r="L75" s="1">
+        <v>454000000000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>4500</v>
       </c>
@@ -5817,8 +6723,20 @@
       <c r="H76" s="2">
         <v>4160000000000</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76">
+        <v>1772000000000</v>
+      </c>
+      <c r="J76">
+        <v>549535000000</v>
+      </c>
+      <c r="K76" s="1">
+        <v>71600000000</v>
+      </c>
+      <c r="L76" s="1">
+        <v>447000000000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>4560</v>
       </c>
@@ -5843,8 +6761,20 @@
       <c r="H77" s="2">
         <v>4170000000000</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I77">
+        <v>1750000000000</v>
+      </c>
+      <c r="J77">
+        <v>638143000000</v>
+      </c>
+      <c r="K77" s="1">
+        <v>68100000000</v>
+      </c>
+      <c r="L77" s="1">
+        <v>441000000000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>4620</v>
       </c>
@@ -5869,8 +6799,20 @@
       <c r="H78" s="2">
         <v>4180000000000</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I78">
+        <v>1734000000000</v>
+      </c>
+      <c r="J78">
+        <v>661034000000</v>
+      </c>
+      <c r="K78" s="1">
+        <v>68100000000</v>
+      </c>
+      <c r="L78" s="1">
+        <v>433000000000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>4680</v>
       </c>
@@ -5895,8 +6837,20 @@
       <c r="H79" s="2">
         <v>4190000000000</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I79">
+        <v>1718000000000</v>
+      </c>
+      <c r="J79">
+        <v>590304000000</v>
+      </c>
+      <c r="K79" s="1">
+        <v>67400000000</v>
+      </c>
+      <c r="L79" s="1">
+        <v>424000000000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>4740</v>
       </c>
@@ -5921,8 +6875,20 @@
       <c r="H80" s="2">
         <v>4200000000000</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I80">
+        <v>1702000000000</v>
+      </c>
+      <c r="J80">
+        <v>548224000000</v>
+      </c>
+      <c r="K80" s="1">
+        <v>64900000000</v>
+      </c>
+      <c r="L80" s="1">
+        <v>415000000000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>4800</v>
       </c>
@@ -5947,8 +6913,20 @@
       <c r="H81" s="2">
         <v>4210000000000</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I81">
+        <v>1686000000000</v>
+      </c>
+      <c r="J81">
+        <v>543938000000</v>
+      </c>
+      <c r="K81" s="1">
+        <v>64700000000</v>
+      </c>
+      <c r="L81" s="1">
+        <v>404000000000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>4860</v>
       </c>
@@ -5973,8 +6951,20 @@
       <c r="H82" s="2">
         <v>4220000000000</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I82">
+        <v>1670000000000</v>
+      </c>
+      <c r="J82">
+        <v>560524000000</v>
+      </c>
+      <c r="K82" s="1">
+        <v>62200000000</v>
+      </c>
+      <c r="L82" s="1">
+        <v>395000000000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>4920</v>
       </c>
@@ -5999,8 +6989,20 @@
       <c r="H83" s="2">
         <v>4228000000000</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I83">
+        <v>1656000000000</v>
+      </c>
+      <c r="J83">
+        <v>559543000000</v>
+      </c>
+      <c r="K83" s="1">
+        <v>63200000000</v>
+      </c>
+      <c r="L83" s="1">
+        <v>391000000000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>4980</v>
       </c>
@@ -6025,8 +7027,20 @@
       <c r="H84" s="2">
         <v>4236000000000</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I84">
+        <v>1642000000000</v>
+      </c>
+      <c r="J84">
+        <v>546862000000</v>
+      </c>
+      <c r="K84" s="1">
+        <v>62000000000</v>
+      </c>
+      <c r="L84" s="1">
+        <v>388000000000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>5040</v>
       </c>
@@ -6051,8 +7065,20 @@
       <c r="H85" s="2">
         <v>4244000000000</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I85">
+        <v>1628000000000</v>
+      </c>
+      <c r="J85">
+        <v>534270000000</v>
+      </c>
+      <c r="K85" s="1">
+        <v>62000000000</v>
+      </c>
+      <c r="L85" s="1">
+        <v>384000000000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>5100</v>
       </c>
@@ -6077,8 +7103,20 @@
       <c r="H86" s="2">
         <v>4252000000000</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I86">
+        <v>1614000000000</v>
+      </c>
+      <c r="J86">
+        <v>556371000000</v>
+      </c>
+      <c r="K86" s="1">
+        <v>59500000000</v>
+      </c>
+      <c r="L86" s="1">
+        <v>377000000000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>5160</v>
       </c>
@@ -6103,8 +7141,20 @@
       <c r="H87" s="2">
         <v>4260000000000</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I87">
+        <v>1600000000000</v>
+      </c>
+      <c r="J87">
+        <v>606189000000</v>
+      </c>
+      <c r="K87" s="1">
+        <v>57600000000</v>
+      </c>
+      <c r="L87" s="1">
+        <v>373000000000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>5220</v>
       </c>
@@ -6129,8 +7179,20 @@
       <c r="H88" s="2">
         <v>4250000000000</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I88">
+        <v>1580000000000</v>
+      </c>
+      <c r="J88">
+        <v>612390000000</v>
+      </c>
+      <c r="K88" s="1">
+        <v>57800000000</v>
+      </c>
+      <c r="L88" s="1">
+        <v>371000000000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>5280</v>
       </c>
@@ -6155,8 +7217,20 @@
       <c r="H89" s="2">
         <v>4240000000000</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I89">
+        <v>1560000000000</v>
+      </c>
+      <c r="J89">
+        <v>635276000000</v>
+      </c>
+      <c r="K89" s="1">
+        <v>56800000000</v>
+      </c>
+      <c r="L89" s="1">
+        <v>369000000000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>5340</v>
       </c>
@@ -6181,8 +7255,20 @@
       <c r="H90" s="2">
         <v>4230000000000</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I90">
+        <v>1540000000000</v>
+      </c>
+      <c r="J90">
+        <v>629627000000</v>
+      </c>
+      <c r="K90" s="1">
+        <v>56100000000</v>
+      </c>
+      <c r="L90" s="1">
+        <v>361000000000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>5400</v>
       </c>
@@ -6207,8 +7293,20 @@
       <c r="H91" s="2">
         <v>4220000000000</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I91">
+        <v>1520000000000</v>
+      </c>
+      <c r="J91">
+        <v>590209000000</v>
+      </c>
+      <c r="K91" s="1">
+        <v>55400000000</v>
+      </c>
+      <c r="L91" s="1">
+        <v>355000000000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>5460</v>
       </c>
@@ -6232,6 +7330,98 @@
       </c>
       <c r="H92" s="2">
         <v>4210000000000</v>
+      </c>
+      <c r="I92">
+        <v>1500000000000</v>
+      </c>
+      <c r="J92">
+        <v>571039000000</v>
+      </c>
+      <c r="K92" s="1">
+        <v>55100000000</v>
+      </c>
+      <c r="L92" s="1">
+        <v>352000000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60206BB5-63D0-9943-A8E8-21A9E6C0DBE3}">
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>23777.923999999999</v>
+      </c>
+      <c r="B1">
+        <v>5959813.6380000003</v>
+      </c>
+      <c r="C1">
+        <v>6599434.875</v>
+      </c>
+      <c r="D1">
+        <v>6468601.3140000002</v>
+      </c>
+      <c r="E1">
+        <v>6179272.4950000001</v>
+      </c>
+      <c r="F1">
+        <v>5916922.4759999998</v>
+      </c>
+      <c r="G1">
+        <v>5640368.3119999999</v>
+      </c>
+      <c r="H1">
+        <v>5396418.0250000004</v>
+      </c>
+      <c r="I1">
+        <v>5195326.7220000001</v>
+      </c>
+      <c r="J1">
+        <v>5054363.415</v>
+      </c>
+      <c r="K1">
+        <v>4865105.2089999998</v>
+      </c>
+      <c r="L1">
+        <v>4770989.9419999998</v>
+      </c>
+      <c r="M1">
+        <v>4607930.45</v>
+      </c>
+      <c r="N1">
+        <v>4441952.8720000004</v>
+      </c>
+      <c r="O1">
+        <v>4329758.7869999995</v>
+      </c>
+      <c r="P1">
+        <v>4213575.9790000003</v>
+      </c>
+      <c r="Q1">
+        <v>4142039.4010000001</v>
+      </c>
+      <c r="R1">
+        <v>4062902.9789999998</v>
+      </c>
+      <c r="S1">
+        <v>3985505.8450000002</v>
+      </c>
+      <c r="T1">
+        <v>3885863.554</v>
+      </c>
+      <c r="U1">
+        <v>3757664.656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>